<commit_message>
fixed weird deaths, still not enough deaths
</commit_message>
<xml_diff>
--- a/modelStructure/RubellaModel.xlsx
+++ b/modelStructure/RubellaModel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taahir/Downloads/RubellaNew/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taahir/Downloads/RubellaNew/modelStructure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF2ABE5-586C-B64E-ADCE-8E77E7F57C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610C88BA-3DC5-694F-8445-1D3725E4C331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="230">
   <si>
     <t>param</t>
   </si>
@@ -587,9 +587,6 @@
     <t>d*M</t>
   </si>
   <si>
-    <t>gamma*I</t>
-  </si>
-  <si>
     <t>v</t>
   </si>
   <si>
@@ -671,12 +668,6 @@
     <t>Births no-maternal-immunity</t>
   </si>
   <si>
-    <t>(1-mprop)*births</t>
-  </si>
-  <si>
-    <t>mprop*births</t>
-  </si>
-  <si>
     <t>lambda*S</t>
   </si>
   <si>
@@ -730,6 +721,15 @@
   <si>
     <t>u*I</t>
   </si>
+  <si>
+    <t>(1-mprop)*bi</t>
+  </si>
+  <si>
+    <t>mprop*bi</t>
+  </si>
+  <si>
+    <t>gamm*I</t>
+  </si>
 </sst>
 </file>
 
@@ -738,7 +738,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;R&quot;#,##0_);[Red]\(&quot;R&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -782,19 +782,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -835,22 +822,19 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1131,13 +1115,13 @@
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1147,7 +1131,7 @@
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="11"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="1"/>
       <c r="D5" s="3"/>
       <c r="F5" s="3"/>
@@ -1160,10 +1144,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C38BB5D-709B-5649-A9CE-CE248A9EEEB9}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1173,23 +1157,23 @@
     <col min="5" max="5" width="37.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>71</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1201,16 +1185,16 @@
         <v>163</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>210</v>
+        <v>227</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
@@ -1221,16 +1205,16 @@
         <v>162</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
@@ -1250,7 +1234,7 @@
         <v>76</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
@@ -1261,27 +1245,27 @@
         <v>164</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>163</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>212</v>
+      <c r="C6" s="3" t="s">
+        <v>209</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>143</v>
@@ -1290,7 +1274,7 @@
         <v>78</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
@@ -1301,7 +1285,7 @@
         <v>170</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>144</v>
@@ -1310,67 +1294,67 @@
         <v>79</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>221</v>
+      <c r="C8" s="3" t="s">
+        <v>218</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>145</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>163</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>222</v>
+      <c r="C9" s="3" t="s">
+        <v>219</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>146</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>168</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>223</v>
+      <c r="C10" s="3" t="s">
+        <v>220</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>147</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
@@ -1381,33 +1365,36 @@
         <v>164</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>165</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>229</v>
+        <v>224</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>226</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
@@ -1418,16 +1405,16 @@
         <v>164</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
@@ -1438,7 +1425,7 @@
         <v>172</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>148</v>
@@ -1447,18 +1434,18 @@
         <v>80</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
         <v>163</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>186</v>
+      <c r="C15" s="3" t="s">
+        <v>185</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>149</v>
@@ -1467,7 +1454,7 @@
         <v>80</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
@@ -1478,7 +1465,7 @@
         <v>172</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>150</v>
@@ -1487,18 +1474,18 @@
         <v>80</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
         <v>170</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>188</v>
+      <c r="C17" s="3" t="s">
+        <v>187</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>151</v>
@@ -1507,7 +1494,7 @@
         <v>80</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
@@ -1518,7 +1505,7 @@
         <v>172</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>152</v>
@@ -1527,28 +1514,32 @@
         <v>80</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
         <v>170</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>226</v>
+      <c r="C19" s="3" t="s">
+        <v>223</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>200</v>
-      </c>
+        <v>199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1570,37 +1561,37 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>180</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>198</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1620,7 +1611,7 @@
       <c r="E2" s="1">
         <v>0</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="7">
         <f t="shared" ref="F2:F13" si="0">1-EXP(-0.95*A2)</f>
         <v>0.61325897654549877</v>
       </c>
@@ -1662,7 +1653,7 @@
       <c r="E3" s="1">
         <v>0</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="7">
         <f t="shared" si="0"/>
         <v>0.85043138077736491</v>
       </c>
@@ -1704,7 +1695,7 @@
       <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="7">
         <f t="shared" si="0"/>
         <v>0.94215567912516152</v>
       </c>
@@ -1746,7 +1737,7 @@
       <c r="E5" s="1">
         <v>0</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="7">
         <f t="shared" si="0"/>
         <v>0.97762922814383435</v>
       </c>
@@ -1788,7 +1779,7 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="7">
         <f t="shared" si="0"/>
         <v>0.99134830479687941</v>
       </c>
@@ -1831,7 +1822,7 @@
         <f>0.847*0.97*0.85</f>
         <v>0.6983514999999999</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="7">
         <f t="shared" si="0"/>
         <v>0.99665403454252877</v>
       </c>
@@ -1873,7 +1864,7 @@
       <c r="E8" s="1">
         <v>0</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="7">
         <f t="shared" si="0"/>
         <v>0.99870597789453419</v>
       </c>
@@ -1915,7 +1906,7 @@
       <c r="E9" s="1">
         <v>0</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="7">
         <f t="shared" si="0"/>
         <v>0.99949954856655943</v>
       </c>
@@ -1957,7 +1948,7 @@
       <c r="E10" s="1">
         <v>0</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="7">
         <f t="shared" si="0"/>
         <v>0.99980645490044195</v>
       </c>
@@ -1999,7 +1990,7 @@
       <c r="E11" s="1">
         <v>0</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="7">
         <f t="shared" si="0"/>
         <v>0.99992514817011235</v>
       </c>
@@ -2041,7 +2032,7 @@
       <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="7">
         <f t="shared" si="0"/>
         <v>0.99997105172670175</v>
       </c>
@@ -2084,7 +2075,7 @@
         <f>0.72*0.97*0.85</f>
         <v>0.59363999999999995</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="7">
         <f t="shared" si="0"/>
         <v>0.99998880451515737</v>
       </c>
@@ -3592,7 +3583,7 @@
       <c r="B50" s="1">
         <v>48</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="C50" s="6" t="s">
         <v>83</v>
       </c>
       <c r="D50" s="1">
@@ -3609,7 +3600,7 @@
         <f>1/365</f>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H50" s="9" t="s">
+      <c r="H50" s="6" t="s">
         <v>83</v>
       </c>
       <c r="I50">
@@ -3674,7 +3665,7 @@
       <c r="B52" s="1">
         <v>72</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C52" s="6" t="s">
         <v>85</v>
       </c>
       <c r="D52" s="1">
@@ -3691,7 +3682,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H52" s="9" t="s">
+      <c r="H52" s="6" t="s">
         <v>85</v>
       </c>
       <c r="I52">
@@ -3756,7 +3747,7 @@
       <c r="B54" s="1">
         <v>96</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C54" s="6" t="s">
         <v>87</v>
       </c>
       <c r="D54" s="1">
@@ -3773,7 +3764,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H54" s="9" t="s">
+      <c r="H54" s="6" t="s">
         <v>87</v>
       </c>
       <c r="I54">
@@ -3838,7 +3829,7 @@
       <c r="B56" s="1">
         <v>120</v>
       </c>
-      <c r="C56" s="9" t="s">
+      <c r="C56" s="6" t="s">
         <v>89</v>
       </c>
       <c r="D56" s="1">
@@ -3855,7 +3846,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H56" s="9" t="s">
+      <c r="H56" s="6" t="s">
         <v>89</v>
       </c>
       <c r="I56">
@@ -3920,7 +3911,7 @@
       <c r="B58" s="1">
         <v>144</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="C58" s="6" t="s">
         <v>91</v>
       </c>
       <c r="D58" s="1">
@@ -3937,7 +3928,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H58" s="9" t="s">
+      <c r="H58" s="6" t="s">
         <v>91</v>
       </c>
       <c r="I58">
@@ -4002,7 +3993,7 @@
       <c r="B60" s="1">
         <v>168</v>
       </c>
-      <c r="C60" s="9" t="s">
+      <c r="C60" s="6" t="s">
         <v>93</v>
       </c>
       <c r="D60" s="1">
@@ -4019,7 +4010,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H60" s="9" t="s">
+      <c r="H60" s="6" t="s">
         <v>93</v>
       </c>
       <c r="I60">
@@ -4084,7 +4075,7 @@
       <c r="B62" s="1">
         <v>192</v>
       </c>
-      <c r="C62" s="9" t="s">
+      <c r="C62" s="6" t="s">
         <v>95</v>
       </c>
       <c r="D62" s="1">
@@ -4101,7 +4092,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H62" s="9" t="s">
+      <c r="H62" s="6" t="s">
         <v>95</v>
       </c>
       <c r="I62">
@@ -4166,7 +4157,7 @@
       <c r="B64" s="1">
         <v>216</v>
       </c>
-      <c r="C64" s="9" t="s">
+      <c r="C64" s="6" t="s">
         <v>97</v>
       </c>
       <c r="D64" s="1">
@@ -4183,7 +4174,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H64" s="9" t="s">
+      <c r="H64" s="6" t="s">
         <v>97</v>
       </c>
       <c r="I64">
@@ -4248,7 +4239,7 @@
       <c r="B66" s="1">
         <v>240</v>
       </c>
-      <c r="C66" s="9" t="s">
+      <c r="C66" s="6" t="s">
         <v>99</v>
       </c>
       <c r="D66" s="1">
@@ -4265,7 +4256,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H66" s="9" t="s">
+      <c r="H66" s="6" t="s">
         <v>99</v>
       </c>
       <c r="I66">
@@ -4330,7 +4321,7 @@
       <c r="B68" s="1">
         <v>264</v>
       </c>
-      <c r="C68" s="9" t="s">
+      <c r="C68" s="6" t="s">
         <v>101</v>
       </c>
       <c r="D68" s="1">
@@ -4347,7 +4338,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H68" s="9" t="s">
+      <c r="H68" s="6" t="s">
         <v>101</v>
       </c>
       <c r="I68">
@@ -4412,7 +4403,7 @@
       <c r="B70" s="1">
         <v>288</v>
       </c>
-      <c r="C70" s="9" t="s">
+      <c r="C70" s="6" t="s">
         <v>103</v>
       </c>
       <c r="D70" s="1">
@@ -4429,7 +4420,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H70" s="9" t="s">
+      <c r="H70" s="6" t="s">
         <v>103</v>
       </c>
       <c r="I70">
@@ -4494,7 +4485,7 @@
       <c r="B72" s="1">
         <v>312</v>
       </c>
-      <c r="C72" s="9" t="s">
+      <c r="C72" s="6" t="s">
         <v>105</v>
       </c>
       <c r="D72" s="1">
@@ -4511,7 +4502,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H72" s="9" t="s">
+      <c r="H72" s="6" t="s">
         <v>105</v>
       </c>
       <c r="I72">
@@ -4576,7 +4567,7 @@
       <c r="B74" s="1">
         <v>336</v>
       </c>
-      <c r="C74" s="9" t="s">
+      <c r="C74" s="6" t="s">
         <v>107</v>
       </c>
       <c r="D74" s="1">
@@ -4593,7 +4584,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H74" s="9" t="s">
+      <c r="H74" s="6" t="s">
         <v>107</v>
       </c>
       <c r="I74">
@@ -4658,7 +4649,7 @@
       <c r="B76" s="1">
         <v>360</v>
       </c>
-      <c r="C76" s="9" t="s">
+      <c r="C76" s="6" t="s">
         <v>109</v>
       </c>
       <c r="D76" s="1">
@@ -4675,7 +4666,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H76" s="9" t="s">
+      <c r="H76" s="6" t="s">
         <v>109</v>
       </c>
       <c r="I76">
@@ -4740,7 +4731,7 @@
       <c r="B78" s="1">
         <v>384</v>
       </c>
-      <c r="C78" s="9" t="s">
+      <c r="C78" s="6" t="s">
         <v>111</v>
       </c>
       <c r="D78" s="1">
@@ -4757,7 +4748,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H78" s="9" t="s">
+      <c r="H78" s="6" t="s">
         <v>111</v>
       </c>
       <c r="I78">
@@ -4822,7 +4813,7 @@
       <c r="B80" s="1">
         <v>408</v>
       </c>
-      <c r="C80" s="9" t="s">
+      <c r="C80" s="6" t="s">
         <v>113</v>
       </c>
       <c r="D80" s="1">
@@ -4839,7 +4830,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H80" s="9" t="s">
+      <c r="H80" s="6" t="s">
         <v>113</v>
       </c>
       <c r="I80">
@@ -4904,7 +4895,7 @@
       <c r="B82" s="1">
         <v>432</v>
       </c>
-      <c r="C82" s="9" t="s">
+      <c r="C82" s="6" t="s">
         <v>115</v>
       </c>
       <c r="D82" s="1">
@@ -4921,7 +4912,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H82" s="9" t="s">
+      <c r="H82" s="6" t="s">
         <v>115</v>
       </c>
       <c r="I82">
@@ -4986,7 +4977,7 @@
       <c r="B84" s="1">
         <v>456</v>
       </c>
-      <c r="C84" s="9" t="s">
+      <c r="C84" s="6" t="s">
         <v>138</v>
       </c>
       <c r="D84" s="1">
@@ -5003,7 +4994,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H84" s="9" t="s">
+      <c r="H84" s="6" t="s">
         <v>138</v>
       </c>
       <c r="I84">
@@ -5068,7 +5059,7 @@
       <c r="B86" s="1">
         <v>480</v>
       </c>
-      <c r="C86" s="9" t="s">
+      <c r="C86" s="6" t="s">
         <v>117</v>
       </c>
       <c r="D86" s="1">
@@ -5085,7 +5076,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H86" s="9" t="s">
+      <c r="H86" s="6" t="s">
         <v>117</v>
       </c>
       <c r="I86">
@@ -5150,7 +5141,7 @@
       <c r="B88" s="1">
         <v>504</v>
       </c>
-      <c r="C88" s="9" t="s">
+      <c r="C88" s="6" t="s">
         <v>119</v>
       </c>
       <c r="D88" s="1">
@@ -5167,7 +5158,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H88" s="9" t="s">
+      <c r="H88" s="6" t="s">
         <v>119</v>
       </c>
       <c r="I88">
@@ -5232,7 +5223,7 @@
       <c r="B90" s="1">
         <v>528</v>
       </c>
-      <c r="C90" s="9" t="s">
+      <c r="C90" s="6" t="s">
         <v>121</v>
       </c>
       <c r="D90" s="1">
@@ -5249,7 +5240,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H90" s="9" t="s">
+      <c r="H90" s="6" t="s">
         <v>121</v>
       </c>
       <c r="I90">
@@ -5314,7 +5305,7 @@
       <c r="B92" s="1">
         <v>552</v>
       </c>
-      <c r="C92" s="9" t="s">
+      <c r="C92" s="6" t="s">
         <v>123</v>
       </c>
       <c r="D92" s="1">
@@ -5331,7 +5322,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H92" s="9" t="s">
+      <c r="H92" s="6" t="s">
         <v>123</v>
       </c>
       <c r="I92">
@@ -5396,7 +5387,7 @@
       <c r="B94" s="1">
         <v>576</v>
       </c>
-      <c r="C94" s="9" t="s">
+      <c r="C94" s="6" t="s">
         <v>125</v>
       </c>
       <c r="D94" s="1">
@@ -5413,7 +5404,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H94" s="9" t="s">
+      <c r="H94" s="6" t="s">
         <v>125</v>
       </c>
       <c r="I94">
@@ -5478,7 +5469,7 @@
       <c r="B96" s="1">
         <v>600</v>
       </c>
-      <c r="C96" s="9" t="s">
+      <c r="C96" s="6" t="s">
         <v>127</v>
       </c>
       <c r="D96" s="1">
@@ -5495,7 +5486,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H96" s="9" t="s">
+      <c r="H96" s="6" t="s">
         <v>127</v>
       </c>
       <c r="I96">
@@ -5560,7 +5551,7 @@
       <c r="B98" s="1">
         <v>624</v>
       </c>
-      <c r="C98" s="9" t="s">
+      <c r="C98" s="6" t="s">
         <v>129</v>
       </c>
       <c r="D98" s="1">
@@ -5577,7 +5568,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H98" s="9" t="s">
+      <c r="H98" s="6" t="s">
         <v>129</v>
       </c>
       <c r="I98">
@@ -5642,7 +5633,7 @@
       <c r="B100" s="1">
         <v>648</v>
       </c>
-      <c r="C100" s="9" t="s">
+      <c r="C100" s="6" t="s">
         <v>131</v>
       </c>
       <c r="D100" s="1">
@@ -5659,7 +5650,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H100" s="9" t="s">
+      <c r="H100" s="6" t="s">
         <v>131</v>
       </c>
       <c r="I100">
@@ -5724,7 +5715,7 @@
       <c r="B102" s="1">
         <v>672</v>
       </c>
-      <c r="C102" s="9" t="s">
+      <c r="C102" s="6" t="s">
         <v>133</v>
       </c>
       <c r="D102" s="1">
@@ -5741,7 +5732,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H102" s="9" t="s">
+      <c r="H102" s="6" t="s">
         <v>133</v>
       </c>
       <c r="I102">
@@ -5806,7 +5797,7 @@
       <c r="B104" s="1">
         <v>696</v>
       </c>
-      <c r="C104" s="9" t="s">
+      <c r="C104" s="6" t="s">
         <v>135</v>
       </c>
       <c r="D104" s="1">
@@ -5823,7 +5814,7 @@
         <f t="shared" si="5"/>
         <v>2.7397260273972603E-3</v>
       </c>
-      <c r="H104" s="9" t="s">
+      <c r="H104" s="6" t="s">
         <v>135</v>
       </c>
       <c r="I104">
@@ -5888,7 +5879,7 @@
       <c r="B106" s="1">
         <v>720</v>
       </c>
-      <c r="C106" s="9" t="s">
+      <c r="C106" s="6" t="s">
         <v>139</v>
       </c>
       <c r="D106" s="1">
@@ -5905,7 +5896,7 @@
         <f>1/3650</f>
         <v>2.7397260273972601E-4</v>
       </c>
-      <c r="H106" s="9" t="s">
+      <c r="H106" s="6" t="s">
         <v>139</v>
       </c>
       <c r="I106">
@@ -5970,7 +5961,7 @@
       <c r="B108" s="1">
         <v>960</v>
       </c>
-      <c r="C108" s="9" t="s">
+      <c r="C108" s="6" t="s">
         <v>141</v>
       </c>
       <c r="D108" s="1">
@@ -5987,7 +5978,7 @@
         <f t="shared" si="8"/>
         <v>2.7397260273972601E-4</v>
       </c>
-      <c r="H108" s="9" t="s">
+      <c r="H108" s="6" t="s">
         <v>141</v>
       </c>
       <c r="I108">
@@ -6012,7 +6003,7 @@
         <v>1080</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D109" s="1">
         <f t="shared" si="7"/>
@@ -6029,7 +6020,7 @@
         <v>2.7397260273972601E-4</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="I109">
         <v>16</v>
@@ -6048,12 +6039,12 @@
     <row r="110" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
-      <c r="C110" s="9"/>
+      <c r="C110" s="6"/>
       <c r="D110" s="3"/>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
       <c r="G110" s="3"/>
-      <c r="H110" s="9"/>
+      <c r="H110" s="6"/>
       <c r="J110" s="1"/>
     </row>
     <row r="111" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6494,187 +6485,187 @@
       <c r="A49" s="1"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A50" s="9"/>
+      <c r="A50" s="6"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A51" s="1"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A52" s="9"/>
+      <c r="A52" s="6"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A53" s="1"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A54" s="9"/>
+      <c r="A54" s="6"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A55" s="1"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A56" s="9"/>
+      <c r="A56" s="6"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A57" s="1"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A58" s="9"/>
+      <c r="A58" s="6"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A59" s="1"/>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A60" s="9"/>
+      <c r="A60" s="6"/>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A61" s="1"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A62" s="9"/>
+      <c r="A62" s="6"/>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A63" s="1"/>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A64" s="9"/>
+      <c r="A64" s="6"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A65" s="1"/>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A66" s="9"/>
+      <c r="A66" s="6"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A67" s="1"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A68" s="9"/>
+      <c r="A68" s="6"/>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A69" s="1"/>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A70" s="9"/>
+      <c r="A70" s="6"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A71" s="1"/>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A72" s="9"/>
+      <c r="A72" s="6"/>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A73" s="1"/>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A74" s="9"/>
+      <c r="A74" s="6"/>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A75" s="1"/>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A76" s="9"/>
+      <c r="A76" s="6"/>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A77" s="1"/>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A78" s="9"/>
+      <c r="A78" s="6"/>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A79" s="1"/>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A80" s="9"/>
+      <c r="A80" s="6"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A81" s="1"/>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A82" s="9"/>
+      <c r="A82" s="6"/>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A83" s="1"/>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A84" s="9"/>
+      <c r="A84" s="6"/>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A85" s="1"/>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A86" s="9"/>
+      <c r="A86" s="6"/>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A87" s="1"/>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A88" s="9"/>
+      <c r="A88" s="6"/>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A89" s="1"/>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A90" s="9"/>
+      <c r="A90" s="6"/>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A91" s="1"/>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A92" s="9"/>
+      <c r="A92" s="6"/>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A93" s="1"/>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A94" s="9"/>
+      <c r="A94" s="6"/>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A95" s="1"/>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A96" s="9"/>
+      <c r="A96" s="6"/>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A97" s="1"/>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A98" s="9"/>
+      <c r="A98" s="6"/>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A99" s="1"/>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A100" s="9"/>
+      <c r="A100" s="6"/>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A101" s="1"/>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A102" s="9"/>
+      <c r="A102" s="6"/>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A103" s="1"/>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A104" s="9"/>
+      <c r="A104" s="6"/>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A105" s="1"/>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A106" s="9"/>
+      <c r="A106" s="6"/>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A107" s="1"/>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A108" s="9"/>
+      <c r="A108" s="6"/>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A109" s="1"/>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A110" s="9"/>
+      <c r="A110" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6685,7 +6676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391ED1A2-F1A6-2F4C-9536-9C7E989709D5}">
   <dimension ref="A1:AF110"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="75" zoomScaleNormal="87" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="87" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -11494,7 +11485,7 @@
       </c>
     </row>
     <row r="50" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="6" t="s">
         <v>83</v>
       </c>
       <c r="B50">
@@ -11690,7 +11681,7 @@
       </c>
     </row>
     <row r="52" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="6" t="s">
         <v>85</v>
       </c>
       <c r="B52">
@@ -11886,7 +11877,7 @@
       </c>
     </row>
     <row r="54" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A54" s="9" t="s">
+      <c r="A54" s="6" t="s">
         <v>87</v>
       </c>
       <c r="B54">
@@ -12082,7 +12073,7 @@
       </c>
     </row>
     <row r="56" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A56" s="9" t="s">
+      <c r="A56" s="6" t="s">
         <v>89</v>
       </c>
       <c r="B56">
@@ -12278,7 +12269,7 @@
       </c>
     </row>
     <row r="58" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="6" t="s">
         <v>91</v>
       </c>
       <c r="B58">
@@ -12474,7 +12465,7 @@
       </c>
     </row>
     <row r="60" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A60" s="9" t="s">
+      <c r="A60" s="6" t="s">
         <v>93</v>
       </c>
       <c r="B60">
@@ -12670,7 +12661,7 @@
       </c>
     </row>
     <row r="62" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A62" s="9" t="s">
+      <c r="A62" s="6" t="s">
         <v>95</v>
       </c>
       <c r="B62">
@@ -12866,7 +12857,7 @@
       </c>
     </row>
     <row r="64" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A64" s="9" t="s">
+      <c r="A64" s="6" t="s">
         <v>97</v>
       </c>
       <c r="B64">
@@ -13062,7 +13053,7 @@
       </c>
     </row>
     <row r="66" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A66" s="9" t="s">
+      <c r="A66" s="6" t="s">
         <v>99</v>
       </c>
       <c r="B66">
@@ -13258,7 +13249,7 @@
       </c>
     </row>
     <row r="68" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A68" s="9" t="s">
+      <c r="A68" s="6" t="s">
         <v>101</v>
       </c>
       <c r="B68">
@@ -13454,7 +13445,7 @@
       </c>
     </row>
     <row r="70" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A70" s="9" t="s">
+      <c r="A70" s="6" t="s">
         <v>103</v>
       </c>
       <c r="B70">
@@ -13650,7 +13641,7 @@
       </c>
     </row>
     <row r="72" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A72" s="9" t="s">
+      <c r="A72" s="6" t="s">
         <v>105</v>
       </c>
       <c r="B72">
@@ -13846,7 +13837,7 @@
       </c>
     </row>
     <row r="74" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A74" s="9" t="s">
+      <c r="A74" s="6" t="s">
         <v>107</v>
       </c>
       <c r="B74">
@@ -14042,7 +14033,7 @@
       </c>
     </row>
     <row r="76" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A76" s="9" t="s">
+      <c r="A76" s="6" t="s">
         <v>109</v>
       </c>
       <c r="B76">
@@ -14238,7 +14229,7 @@
       </c>
     </row>
     <row r="78" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A78" s="9" t="s">
+      <c r="A78" s="6" t="s">
         <v>111</v>
       </c>
       <c r="B78">
@@ -14434,7 +14425,7 @@
       </c>
     </row>
     <row r="80" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A80" s="9" t="s">
+      <c r="A80" s="6" t="s">
         <v>113</v>
       </c>
       <c r="B80">
@@ -14630,7 +14621,7 @@
       </c>
     </row>
     <row r="82" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A82" s="9" t="s">
+      <c r="A82" s="6" t="s">
         <v>115</v>
       </c>
       <c r="B82">
@@ -14826,7 +14817,7 @@
       </c>
     </row>
     <row r="84" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A84" s="9" t="s">
+      <c r="A84" s="6" t="s">
         <v>138</v>
       </c>
       <c r="B84">
@@ -15022,7 +15013,7 @@
       </c>
     </row>
     <row r="86" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A86" s="9" t="s">
+      <c r="A86" s="6" t="s">
         <v>117</v>
       </c>
       <c r="B86">
@@ -15218,7 +15209,7 @@
       </c>
     </row>
     <row r="88" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A88" s="9" t="s">
+      <c r="A88" s="6" t="s">
         <v>119</v>
       </c>
       <c r="B88">
@@ -15414,7 +15405,7 @@
       </c>
     </row>
     <row r="90" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A90" s="9" t="s">
+      <c r="A90" s="6" t="s">
         <v>121</v>
       </c>
       <c r="B90">
@@ -15610,7 +15601,7 @@
       </c>
     </row>
     <row r="92" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A92" s="9" t="s">
+      <c r="A92" s="6" t="s">
         <v>123</v>
       </c>
       <c r="B92">
@@ -15806,7 +15797,7 @@
       </c>
     </row>
     <row r="94" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A94" s="9" t="s">
+      <c r="A94" s="6" t="s">
         <v>125</v>
       </c>
       <c r="B94">
@@ -16002,7 +15993,7 @@
       </c>
     </row>
     <row r="96" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A96" s="9" t="s">
+      <c r="A96" s="6" t="s">
         <v>127</v>
       </c>
       <c r="B96">
@@ -16198,7 +16189,7 @@
       </c>
     </row>
     <row r="98" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A98" s="9" t="s">
+      <c r="A98" s="6" t="s">
         <v>129</v>
       </c>
       <c r="B98">
@@ -16394,7 +16385,7 @@
       </c>
     </row>
     <row r="100" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A100" s="9" t="s">
+      <c r="A100" s="6" t="s">
         <v>131</v>
       </c>
       <c r="B100">
@@ -16590,7 +16581,7 @@
       </c>
     </row>
     <row r="102" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A102" s="9" t="s">
+      <c r="A102" s="6" t="s">
         <v>133</v>
       </c>
       <c r="B102">
@@ -16786,7 +16777,7 @@
       </c>
     </row>
     <row r="104" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A104" s="9" t="s">
+      <c r="A104" s="6" t="s">
         <v>135</v>
       </c>
       <c r="B104">
@@ -16982,7 +16973,7 @@
       </c>
     </row>
     <row r="106" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A106" s="9" t="s">
+      <c r="A106" s="6" t="s">
         <v>158</v>
       </c>
       <c r="B106">
@@ -17178,7 +17169,7 @@
       </c>
     </row>
     <row r="108" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A108" s="9" t="s">
+      <c r="A108" s="6" t="s">
         <v>160</v>
       </c>
       <c r="B108">
@@ -17277,7 +17268,7 @@
     </row>
     <row r="109" spans="1:32" x14ac:dyDescent="0.15">
       <c r="A109" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B109">
         <v>0.19442177668345256</v>
@@ -17374,7 +17365,7 @@
       </c>
     </row>
     <row r="110" spans="1:32" x14ac:dyDescent="0.15">
-      <c r="A110" s="9"/>
+      <c r="A110" s="6"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AF110">
@@ -17656,187 +17647,187 @@
       <c r="AW1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AX1" s="9" t="s">
+      <c r="AX1" s="6" t="s">
         <v>83</v>
       </c>
       <c r="AY1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AZ1" s="9" t="s">
+      <c r="AZ1" s="6" t="s">
         <v>85</v>
       </c>
       <c r="BA1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="BB1" s="9" t="s">
+      <c r="BB1" s="6" t="s">
         <v>87</v>
       </c>
       <c r="BC1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="BD1" s="9" t="s">
+      <c r="BD1" s="6" t="s">
         <v>89</v>
       </c>
       <c r="BE1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="BF1" s="9" t="s">
+      <c r="BF1" s="6" t="s">
         <v>91</v>
       </c>
       <c r="BG1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="BH1" s="9" t="s">
+      <c r="BH1" s="6" t="s">
         <v>93</v>
       </c>
       <c r="BI1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="BJ1" s="9" t="s">
+      <c r="BJ1" s="6" t="s">
         <v>95</v>
       </c>
       <c r="BK1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="BL1" s="9" t="s">
+      <c r="BL1" s="6" t="s">
         <v>97</v>
       </c>
       <c r="BM1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="BN1" s="9" t="s">
+      <c r="BN1" s="6" t="s">
         <v>99</v>
       </c>
       <c r="BO1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="BP1" s="9" t="s">
+      <c r="BP1" s="6" t="s">
         <v>101</v>
       </c>
       <c r="BQ1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="BR1" s="9" t="s">
+      <c r="BR1" s="6" t="s">
         <v>103</v>
       </c>
       <c r="BS1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="BT1" s="9" t="s">
+      <c r="BT1" s="6" t="s">
         <v>105</v>
       </c>
       <c r="BU1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="BV1" s="9" t="s">
+      <c r="BV1" s="6" t="s">
         <v>107</v>
       </c>
       <c r="BW1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="BX1" s="9" t="s">
+      <c r="BX1" s="6" t="s">
         <v>109</v>
       </c>
       <c r="BY1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="BZ1" s="9" t="s">
+      <c r="BZ1" s="6" t="s">
         <v>111</v>
       </c>
       <c r="CA1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="CB1" s="9" t="s">
+      <c r="CB1" s="6" t="s">
         <v>113</v>
       </c>
       <c r="CC1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="CD1" s="9" t="s">
+      <c r="CD1" s="6" t="s">
         <v>115</v>
       </c>
       <c r="CE1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="CF1" s="9" t="s">
+      <c r="CF1" s="6" t="s">
         <v>138</v>
       </c>
       <c r="CG1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="CH1" s="9" t="s">
+      <c r="CH1" s="6" t="s">
         <v>117</v>
       </c>
       <c r="CI1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="CJ1" s="9" t="s">
+      <c r="CJ1" s="6" t="s">
         <v>119</v>
       </c>
       <c r="CK1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="CL1" s="9" t="s">
+      <c r="CL1" s="6" t="s">
         <v>121</v>
       </c>
       <c r="CM1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="CN1" s="9" t="s">
+      <c r="CN1" s="6" t="s">
         <v>123</v>
       </c>
       <c r="CO1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="CP1" s="9" t="s">
+      <c r="CP1" s="6" t="s">
         <v>125</v>
       </c>
       <c r="CQ1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="CR1" s="9" t="s">
+      <c r="CR1" s="6" t="s">
         <v>127</v>
       </c>
       <c r="CS1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="CT1" s="9" t="s">
+      <c r="CT1" s="6" t="s">
         <v>129</v>
       </c>
       <c r="CU1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="CV1" s="9" t="s">
+      <c r="CV1" s="6" t="s">
         <v>131</v>
       </c>
       <c r="CW1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="CX1" s="9" t="s">
+      <c r="CX1" s="6" t="s">
         <v>133</v>
       </c>
       <c r="CY1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="CZ1" s="9" t="s">
+      <c r="CZ1" s="6" t="s">
         <v>135</v>
       </c>
       <c r="DA1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="DB1" s="9" t="s">
+      <c r="DB1" s="6" t="s">
         <v>139</v>
       </c>
       <c r="DC1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="DD1" s="9" t="s">
+      <c r="DD1" s="6" t="s">
         <v>141</v>
       </c>
       <c r="DE1" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="DF1" s="9"/>
+        <v>215</v>
+      </c>
+      <c r="DF1" s="6"/>
     </row>
     <row r="2" spans="1:110" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
@@ -33631,7 +33622,7 @@
       </c>
     </row>
     <row r="50" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="6" t="s">
         <v>83</v>
       </c>
       <c r="B50">
@@ -34289,7 +34280,7 @@
       </c>
     </row>
     <row r="52" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="6" t="s">
         <v>85</v>
       </c>
       <c r="B52">
@@ -34947,7 +34938,7 @@
       </c>
     </row>
     <row r="54" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="9" t="s">
+      <c r="A54" s="6" t="s">
         <v>87</v>
       </c>
       <c r="B54">
@@ -35605,7 +35596,7 @@
       </c>
     </row>
     <row r="56" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="9" t="s">
+      <c r="A56" s="6" t="s">
         <v>89</v>
       </c>
       <c r="B56">
@@ -36263,7 +36254,7 @@
       </c>
     </row>
     <row r="58" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="6" t="s">
         <v>91</v>
       </c>
       <c r="B58">
@@ -36921,7 +36912,7 @@
       </c>
     </row>
     <row r="60" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="9" t="s">
+      <c r="A60" s="6" t="s">
         <v>93</v>
       </c>
       <c r="B60">
@@ -37579,7 +37570,7 @@
       </c>
     </row>
     <row r="62" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="9" t="s">
+      <c r="A62" s="6" t="s">
         <v>95</v>
       </c>
       <c r="B62">
@@ -38237,7 +38228,7 @@
       </c>
     </row>
     <row r="64" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="9" t="s">
+      <c r="A64" s="6" t="s">
         <v>97</v>
       </c>
       <c r="B64">
@@ -38895,7 +38886,7 @@
       </c>
     </row>
     <row r="66" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="9" t="s">
+      <c r="A66" s="6" t="s">
         <v>99</v>
       </c>
       <c r="B66">
@@ -39553,7 +39544,7 @@
       </c>
     </row>
     <row r="68" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="9" t="s">
+      <c r="A68" s="6" t="s">
         <v>101</v>
       </c>
       <c r="B68">
@@ -40211,7 +40202,7 @@
       </c>
     </row>
     <row r="70" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="9" t="s">
+      <c r="A70" s="6" t="s">
         <v>103</v>
       </c>
       <c r="B70">
@@ -40869,7 +40860,7 @@
       </c>
     </row>
     <row r="72" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="9" t="s">
+      <c r="A72" s="6" t="s">
         <v>105</v>
       </c>
       <c r="B72">
@@ -41527,7 +41518,7 @@
       </c>
     </row>
     <row r="74" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="9" t="s">
+      <c r="A74" s="6" t="s">
         <v>107</v>
       </c>
       <c r="B74">
@@ -42185,7 +42176,7 @@
       </c>
     </row>
     <row r="76" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="9" t="s">
+      <c r="A76" s="6" t="s">
         <v>109</v>
       </c>
       <c r="B76">
@@ -42843,7 +42834,7 @@
       </c>
     </row>
     <row r="78" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="9" t="s">
+      <c r="A78" s="6" t="s">
         <v>111</v>
       </c>
       <c r="B78">
@@ -43501,7 +43492,7 @@
       </c>
     </row>
     <row r="80" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="9" t="s">
+      <c r="A80" s="6" t="s">
         <v>113</v>
       </c>
       <c r="B80">
@@ -44159,7 +44150,7 @@
       </c>
     </row>
     <row r="82" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="9" t="s">
+      <c r="A82" s="6" t="s">
         <v>115</v>
       </c>
       <c r="B82">
@@ -44817,7 +44808,7 @@
       </c>
     </row>
     <row r="84" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="9" t="s">
+      <c r="A84" s="6" t="s">
         <v>138</v>
       </c>
       <c r="B84">
@@ -45475,7 +45466,7 @@
       </c>
     </row>
     <row r="86" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A86" s="9" t="s">
+      <c r="A86" s="6" t="s">
         <v>117</v>
       </c>
       <c r="B86">
@@ -46133,7 +46124,7 @@
       </c>
     </row>
     <row r="88" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="9" t="s">
+      <c r="A88" s="6" t="s">
         <v>119</v>
       </c>
       <c r="B88">
@@ -46791,7 +46782,7 @@
       </c>
     </row>
     <row r="90" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A90" s="9" t="s">
+      <c r="A90" s="6" t="s">
         <v>121</v>
       </c>
       <c r="B90">
@@ -47449,7 +47440,7 @@
       </c>
     </row>
     <row r="92" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A92" s="9" t="s">
+      <c r="A92" s="6" t="s">
         <v>123</v>
       </c>
       <c r="B92">
@@ -48107,7 +48098,7 @@
       </c>
     </row>
     <row r="94" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A94" s="9" t="s">
+      <c r="A94" s="6" t="s">
         <v>125</v>
       </c>
       <c r="B94">
@@ -48765,7 +48756,7 @@
       </c>
     </row>
     <row r="96" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A96" s="9" t="s">
+      <c r="A96" s="6" t="s">
         <v>127</v>
       </c>
       <c r="B96">
@@ -49423,7 +49414,7 @@
       </c>
     </row>
     <row r="98" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="9" t="s">
+      <c r="A98" s="6" t="s">
         <v>129</v>
       </c>
       <c r="B98">
@@ -50081,7 +50072,7 @@
       </c>
     </row>
     <row r="100" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A100" s="9" t="s">
+      <c r="A100" s="6" t="s">
         <v>131</v>
       </c>
       <c r="B100">
@@ -50739,7 +50730,7 @@
       </c>
     </row>
     <row r="102" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A102" s="9" t="s">
+      <c r="A102" s="6" t="s">
         <v>133</v>
       </c>
       <c r="B102">
@@ -51397,7 +51388,7 @@
       </c>
     </row>
     <row r="104" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A104" s="9" t="s">
+      <c r="A104" s="6" t="s">
         <v>135</v>
       </c>
       <c r="B104">
@@ -52055,7 +52046,7 @@
       </c>
     </row>
     <row r="106" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A106" s="9" t="s">
+      <c r="A106" s="6" t="s">
         <v>139</v>
       </c>
       <c r="B106">
@@ -52713,7 +52704,7 @@
       </c>
     </row>
     <row r="108" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A108" s="9" t="s">
+      <c r="A108" s="6" t="s">
         <v>141</v>
       </c>
       <c r="B108">
@@ -53043,7 +53034,7 @@
     </row>
     <row r="109" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A109" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B109">
         <v>0.27893747218213799</v>
@@ -53371,7 +53362,7 @@
       </c>
     </row>
     <row r="110" spans="1:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A110" s="9"/>
+      <c r="A110" s="6"/>
     </row>
     <row r="113" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B113" s="5" t="s">

</xml_diff>

<commit_message>
Fertility based births, R0, E compartment fix 1
</commit_message>
<xml_diff>
--- a/modelStructure/RubellaModel.xlsx
+++ b/modelStructure/RubellaModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taahir/Downloads/RubellaNew/modelStructure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6315CE2A-0AD0-4049-AAEA-E4001FE3D305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F015C6EA-6AA5-1B49-8071-D0604516623B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="universal" sheetId="1" r:id="rId1"/>
@@ -813,9 +813,6 @@
     <t>Edeath</t>
   </si>
   <si>
-    <t>alpha*I</t>
-  </si>
-  <si>
     <t>Infec</t>
   </si>
   <si>
@@ -1030,6 +1027,9 @@
   </si>
   <si>
     <t>70+</t>
+  </si>
+  <si>
+    <t>alpha*E</t>
   </si>
 </sst>
 </file>
@@ -1456,8 +1456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17953FCA-C542-F245-8458-E0A08348AC2A}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1798,13 +1798,13 @@
         <v>162</v>
       </c>
       <c r="C17" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="E17" s="9" t="s">
         <v>258</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>259</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>223</v>
@@ -1815,16 +1815,16 @@
         <v>234</v>
       </c>
       <c r="B18" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="D18" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="E18" s="9" t="s">
         <v>262</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>263</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>223</v>
@@ -1858,10 +1858,10 @@
         <v>169</v>
       </c>
       <c r="C20" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>264</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>265</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>78</v>
@@ -1878,13 +1878,13 @@
         <v>208</v>
       </c>
       <c r="C21" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="E21" s="9" t="s">
         <v>267</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>268</v>
       </c>
       <c r="F21" s="9" t="s">
         <v>223</v>
@@ -1898,10 +1898,10 @@
         <v>169</v>
       </c>
       <c r="C22" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>269</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>270</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>78</v>
@@ -1918,13 +1918,13 @@
         <v>166</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>143</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>223</v>
@@ -1938,13 +1938,13 @@
         <v>226</v>
       </c>
       <c r="C24" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="E24" s="9" t="s">
         <v>274</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>275</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>223</v>
@@ -1958,13 +1958,13 @@
         <v>247</v>
       </c>
       <c r="C25" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="E25" s="9" t="s">
         <v>277</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>278</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>223</v>
@@ -1972,16 +1972,16 @@
     </row>
     <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>169</v>
       </c>
       <c r="C26" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>280</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>281</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>78</v>
@@ -1992,19 +1992,19 @@
     </row>
     <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>226</v>
       </c>
       <c r="C27" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="E27" s="9" t="s">
         <v>283</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>284</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>223</v>
@@ -2012,19 +2012,19 @@
     </row>
     <row r="28" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>247</v>
       </c>
       <c r="C28" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="E28" s="9" t="s">
         <v>286</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>287</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>223</v>
@@ -2032,16 +2032,16 @@
     </row>
     <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>169</v>
       </c>
       <c r="C29" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>289</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>290</v>
       </c>
       <c r="E29" s="9" t="s">
         <v>78</v>
@@ -2052,19 +2052,19 @@
     </row>
     <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>230</v>
       </c>
       <c r="C30" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="D30" s="9" t="s">
-        <v>292</v>
-      </c>
       <c r="E30" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>223</v>
@@ -2072,19 +2072,19 @@
     </row>
     <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>234</v>
       </c>
       <c r="C31" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="E31" s="9" t="s">
         <v>294</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>295</v>
       </c>
       <c r="F31" s="9" t="s">
         <v>223</v>
@@ -2092,19 +2092,19 @@
     </row>
     <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>251</v>
       </c>
       <c r="C32" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="D32" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="E32" s="9" t="s">
         <v>297</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>298</v>
       </c>
       <c r="F32" s="9" t="s">
         <v>223</v>
@@ -2112,19 +2112,19 @@
     </row>
     <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>247</v>
       </c>
       <c r="C33" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="D33" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="E33" s="9" t="s">
         <v>300</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>301</v>
       </c>
       <c r="F33" s="9" t="s">
         <v>223</v>
@@ -2132,16 +2132,16 @@
     </row>
     <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>169</v>
       </c>
       <c r="C34" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="D34" s="9" t="s">
         <v>303</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>304</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>78</v>
@@ -2152,19 +2152,19 @@
     </row>
     <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>247</v>
       </c>
       <c r="C35" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="D35" s="9" t="s">
         <v>305</v>
       </c>
-      <c r="D35" s="9" t="s">
-        <v>306</v>
-      </c>
       <c r="E35" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F35" s="9" t="s">
         <v>223</v>
@@ -2172,16 +2172,16 @@
     </row>
     <row r="36" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>169</v>
       </c>
       <c r="C36" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="D36" s="9" t="s">
         <v>308</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>309</v>
       </c>
       <c r="E36" s="9" t="s">
         <v>78</v>
@@ -2192,19 +2192,19 @@
     </row>
     <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>251</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F37" s="9" t="s">
         <v>223</v>
@@ -2212,19 +2212,19 @@
     </row>
     <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>234</v>
       </c>
       <c r="C38" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="D38" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="D38" s="9" t="s">
-        <v>312</v>
-      </c>
       <c r="E38" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F38" s="9" t="s">
         <v>223</v>
@@ -2646,7 +2646,7 @@
   </sheetPr>
   <dimension ref="A1:J138"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
+    <sheetView zoomScale="116" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -2689,7 +2689,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D2" s="2">
         <f>365/180</f>
@@ -2700,7 +2700,7 @@
         <v>2.0277777777777777</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -2709,7 +2709,7 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <f>H2/120</f>
+        <f t="shared" ref="I2:I33" si="0">H2/120</f>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J2">
@@ -2724,7 +2724,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D3" s="2">
         <f>365/180</f>
@@ -2735,7 +2735,7 @@
         <v>2.0277777777777777</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -2744,7 +2744,7 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <f>H3/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J3">
@@ -2759,7 +2759,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2768,7 +2768,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -2777,7 +2777,7 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <f>H4/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J4">
@@ -2792,7 +2792,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2801,7 +2801,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -2810,7 +2810,7 @@
         <v>1</v>
       </c>
       <c r="I5">
-        <f>H5/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J5">
@@ -2825,7 +2825,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -2834,7 +2834,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -2843,7 +2843,7 @@
         <v>1</v>
       </c>
       <c r="I6">
-        <f>H6/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J6">
@@ -2876,7 +2876,7 @@
         <v>1</v>
       </c>
       <c r="I7">
-        <f>H7/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J7">
@@ -2909,7 +2909,7 @@
         <v>1</v>
       </c>
       <c r="I8">
-        <f>H8/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J8">
@@ -2942,7 +2942,7 @@
         <v>1</v>
       </c>
       <c r="I9">
-        <f>H9/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J9">
@@ -2975,7 +2975,7 @@
         <v>1</v>
       </c>
       <c r="I10">
-        <f>H10/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J10">
@@ -3008,7 +3008,7 @@
         <v>1</v>
       </c>
       <c r="I11">
-        <f>H11/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J11">
@@ -3041,7 +3041,7 @@
         <v>1</v>
       </c>
       <c r="I12">
-        <f>H12/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J12">
@@ -3074,7 +3074,7 @@
         <v>1</v>
       </c>
       <c r="I13">
-        <f>H13/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J13">
@@ -3107,7 +3107,7 @@
         <v>1</v>
       </c>
       <c r="I14">
-        <f>H14/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J14">
@@ -3140,7 +3140,7 @@
         <v>1</v>
       </c>
       <c r="I15">
-        <f>H15/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J15">
@@ -3173,7 +3173,7 @@
         <v>1</v>
       </c>
       <c r="I16">
-        <f>H16/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J16">
@@ -3206,7 +3206,7 @@
         <v>1</v>
       </c>
       <c r="I17">
-        <f>H17/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J17">
@@ -3239,7 +3239,7 @@
         <v>1</v>
       </c>
       <c r="I18">
-        <f>H18/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J18">
@@ -3272,7 +3272,7 @@
         <v>1</v>
       </c>
       <c r="I19">
-        <f>H19/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J19">
@@ -3305,7 +3305,7 @@
         <v>1</v>
       </c>
       <c r="I20">
-        <f>H20/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J20">
@@ -3338,7 +3338,7 @@
         <v>1</v>
       </c>
       <c r="I21">
-        <f>H21/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J21">
@@ -3371,7 +3371,7 @@
         <v>1</v>
       </c>
       <c r="I22">
-        <f>H22/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J22">
@@ -3404,7 +3404,7 @@
         <v>1</v>
       </c>
       <c r="I23">
-        <f>H23/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J23">
@@ -3437,7 +3437,7 @@
         <v>1</v>
       </c>
       <c r="I24">
-        <f>H24/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J24">
@@ -3470,7 +3470,7 @@
         <v>1</v>
       </c>
       <c r="I25">
-        <f>H25/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J25">
@@ -3503,7 +3503,7 @@
         <v>1</v>
       </c>
       <c r="I26">
-        <f>H26/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J26">
@@ -3536,7 +3536,7 @@
         <v>1</v>
       </c>
       <c r="I27">
-        <f>H27/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J27">
@@ -3569,7 +3569,7 @@
         <v>1</v>
       </c>
       <c r="I28">
-        <f>H28/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J28">
@@ -3602,7 +3602,7 @@
         <v>1</v>
       </c>
       <c r="I29">
-        <f>H29/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J29">
@@ -3635,7 +3635,7 @@
         <v>1</v>
       </c>
       <c r="I30">
-        <f>H30/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J30">
@@ -3668,7 +3668,7 @@
         <v>1</v>
       </c>
       <c r="I31">
-        <f>H31/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J31">
@@ -3701,7 +3701,7 @@
         <v>1</v>
       </c>
       <c r="I32">
-        <f>H32/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J32">
@@ -3734,7 +3734,7 @@
         <v>1</v>
       </c>
       <c r="I33">
-        <f>H33/120</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J33">
@@ -3767,7 +3767,7 @@
         <v>1</v>
       </c>
       <c r="I34">
-        <f>H34/120</f>
+        <f t="shared" ref="I34:I65" si="1">H34/120</f>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J34">
@@ -3800,7 +3800,7 @@
         <v>1</v>
       </c>
       <c r="I35">
-        <f>H35/120</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J35">
@@ -3833,7 +3833,7 @@
         <v>1</v>
       </c>
       <c r="I36">
-        <f>H36/120</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J36">
@@ -3866,7 +3866,7 @@
         <v>1</v>
       </c>
       <c r="I37">
-        <f>H37/120</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J37">
@@ -3899,7 +3899,7 @@
         <v>1</v>
       </c>
       <c r="I38">
-        <f>H38/120</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J38">
@@ -3932,7 +3932,7 @@
         <v>1</v>
       </c>
       <c r="I39">
-        <f>H39/120</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J39">
@@ -3965,7 +3965,7 @@
         <v>1</v>
       </c>
       <c r="I40">
-        <f>H40/120</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J40">
@@ -3998,7 +3998,7 @@
         <v>1</v>
       </c>
       <c r="I41">
-        <f>H41/120</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J41">
@@ -4031,7 +4031,7 @@
         <v>1</v>
       </c>
       <c r="I42">
-        <f>H42/120</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J42">
@@ -4064,7 +4064,7 @@
         <v>1</v>
       </c>
       <c r="I43">
-        <f>H43/120</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J43">
@@ -4097,7 +4097,7 @@
         <v>1</v>
       </c>
       <c r="I44">
-        <f>H44/120</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J44">
@@ -4130,7 +4130,7 @@
         <v>1</v>
       </c>
       <c r="I45">
-        <f>H45/120</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J45">
@@ -4163,7 +4163,7 @@
         <v>1</v>
       </c>
       <c r="I46">
-        <f>H46/120</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J46">
@@ -4196,7 +4196,7 @@
         <v>1</v>
       </c>
       <c r="I47">
-        <f>H47/120</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J47">
@@ -4229,7 +4229,7 @@
         <v>1</v>
       </c>
       <c r="I48">
-        <f>H48/120</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J48">
@@ -4244,7 +4244,7 @@
         <v>47</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -4253,7 +4253,7 @@
         <v>1</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G49">
         <v>10</v>
@@ -4262,7 +4262,7 @@
         <v>1</v>
       </c>
       <c r="I49">
-        <f>H49/120</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="J49">
@@ -4295,7 +4295,7 @@
         <v>12</v>
       </c>
       <c r="I50">
-        <f>H50/120</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="J50">
@@ -4328,7 +4328,7 @@
         <v>12</v>
       </c>
       <c r="I51">
-        <f>H51/120</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="J51">
@@ -4361,7 +4361,7 @@
         <v>12</v>
       </c>
       <c r="I52">
-        <f>H52/120</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="J52">
@@ -4394,7 +4394,7 @@
         <v>12</v>
       </c>
       <c r="I53">
-        <f>H53/120</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="J53">
@@ -4427,7 +4427,7 @@
         <v>12</v>
       </c>
       <c r="I54">
-        <f>H54/120</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="J54">
@@ -4460,7 +4460,7 @@
         <v>12</v>
       </c>
       <c r="I55">
-        <f>H55/120</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="J55">
@@ -4493,7 +4493,7 @@
         <v>12</v>
       </c>
       <c r="I56">
-        <f>H56/120</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="J56">
@@ -4526,7 +4526,7 @@
         <v>12</v>
       </c>
       <c r="I57">
-        <f>H57/120</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="J57">
@@ -4559,7 +4559,7 @@
         <v>12</v>
       </c>
       <c r="I58">
-        <f>H58/120</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="J58">
@@ -4592,7 +4592,7 @@
         <v>12</v>
       </c>
       <c r="I59">
-        <f>H59/120</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="J59">
@@ -4625,7 +4625,7 @@
         <v>12</v>
       </c>
       <c r="I60">
-        <f>H60/120</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="J60">
@@ -4658,7 +4658,7 @@
         <v>12</v>
       </c>
       <c r="I61">
-        <f>H61/120</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="J61">
@@ -4691,7 +4691,7 @@
         <v>12</v>
       </c>
       <c r="I62">
-        <f>H62/120</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="J62">
@@ -4724,7 +4724,7 @@
         <v>12</v>
       </c>
       <c r="I63">
-        <f>H63/120</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="J63">
@@ -4739,7 +4739,7 @@
         <v>216</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D64">
         <f>365/(265*30)</f>
@@ -4750,7 +4750,7 @@
         <v>4.5911949685534588E-2</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G64">
         <v>14</v>
@@ -4759,7 +4759,7 @@
         <v>12</v>
       </c>
       <c r="I64">
-        <f>H64/120</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="J64">
@@ -16672,10 +16672,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>314</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
@@ -16705,10 +16705,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -16716,10 +16716,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
@@ -16727,10 +16727,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C9" t="b">
         <v>1</v>
@@ -16738,10 +16738,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>

</xml_diff>